<commit_message>
subiendo version para presentar, sube a base de datos
</commit_message>
<xml_diff>
--- a/ejemplo_excel/ejemplo_datos_banco.xlsx
+++ b/ejemplo_excel/ejemplo_datos_banco.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayay\Documents\ACC\SEPTIEMBRE\SERVICIOS_BANCO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayay\Documents\ACC\SEPTIEMBRE\SERVICIOS_BANCO\codigo\ejemplo_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91598F5C-0EF3-4FA1-B45E-1C4585FD8BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C2E1D0-34D4-4B3A-8656-FDC2EF7256FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="2571" windowWidth="16200" windowHeight="9969" xr2:uid="{71856ACC-7502-4058-8ADD-A6BAE6DFB31F}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="21806" windowHeight="13886" xr2:uid="{71856ACC-7502-4058-8ADD-A6BAE6DFB31F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -168,7 +168,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;\ #,##0;[Red]\-&quot;$&quot;\ #,##0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +203,13 @@
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -225,7 +232,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -240,6 +247,8 @@
     <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -575,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21F3F83A-A166-4F1D-AC93-532D484AEFD8}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.35"/>
@@ -588,9 +597,9 @@
     <col min="3" max="3" width="13" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.15234375" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.23046875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.3828125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.3828125" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.4609375" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.69140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.69140625" style="8" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="11.07421875" style="4"/>
   </cols>
   <sheetData>
@@ -610,13 +619,13 @@
       <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="4" t="s">
@@ -639,7 +648,7 @@
       <c r="E2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="8">
         <v>234532</v>
       </c>
       <c r="G2" s="7" t="s">
@@ -665,10 +674,10 @@
       <c r="E3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="8">
         <v>436423</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="8">
         <v>31245234234</v>
       </c>
       <c r="I3" s="4" t="s">
@@ -691,7 +700,7 @@
       <c r="E4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="8">
         <v>435314</v>
       </c>
       <c r="I4" s="4" t="s">
@@ -714,10 +723,10 @@
       <c r="E5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="8">
         <v>1235563</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="8">
         <v>342342342</v>
       </c>
       <c r="I5" s="4" t="s">
@@ -740,7 +749,7 @@
       <c r="E6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="8">
         <v>54353452</v>
       </c>
       <c r="I6" s="4" t="s">
@@ -763,7 +772,7 @@
       <c r="E7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="8">
         <v>2342523</v>
       </c>
       <c r="G7" s="7" t="s">
@@ -789,7 +798,7 @@
       <c r="E8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="8">
         <v>3241234</v>
       </c>
       <c r="I8" s="4" t="s">
@@ -812,7 +821,7 @@
       <c r="E9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="8">
         <v>546653</v>
       </c>
       <c r="I9" s="4" t="s">
@@ -835,7 +844,7 @@
       <c r="E10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="8">
         <v>435234</v>
       </c>
       <c r="G10" s="7" t="s">
@@ -844,6 +853,9 @@
       <c r="I10" s="4" t="s">
         <v>39</v>
       </c>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F19" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>